<commit_message>
Modified Excel & SQL Utilities
</commit_message>
<xml_diff>
--- a/src/main/resources/testData/testData.xlsx
+++ b/src/main/resources/testData/testData.xlsx
@@ -4,15 +4,14 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -20,81 +19,26 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>Name</t>
+    <t>John Wick</t>
   </si>
   <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Current Address</t>
-  </si>
-  <si>
-    <t>Permenant Address</t>
-  </si>
-  <si>
-    <t>Sachin Taware</t>
-  </si>
-  <si>
-    <t>sachintaw@cybage.com</t>
-  </si>
-  <si>
-    <t>Manjri, Pune</t>
-  </si>
-  <si>
-    <t>Loni, Ahmednager</t>
-  </si>
-  <si>
-    <t>Dinesh Gouda</t>
-  </si>
-  <si>
-    <t>dineshgo@cybage.com</t>
-  </si>
-  <si>
-    <t>VimanNagar, Pune</t>
-  </si>
-  <si>
-    <t>Odisha,India</t>
-  </si>
-  <si>
-    <t>Lorem Ipsum is simply dummy text of the printing and typesetting industry. Lorem Ipsum has been the industry's standard dummy text ever since the 1500s, when an unknown printer took a galley of type and scrambled it to make a type specimen book. It has survived not only five centuries, but also the leap into electronic typesetting, remaining essentially unchanged. It was popularised in the 1960s with the release of Letraset sheets containing Lorem Ipsum passages, and more recently with desktop publishing software like Aldus PageMaker including versions of Lorem Ipsum.</t>
-  </si>
-  <si>
-    <t>It is a long established fact that a reader will be distracted by the readable content of a page when looking at its layout. The point of using Lorem Ipsum is that it has a more-or-less normal distribution of letters, as opposed to using 'Content here, content here', making it look like readable English. Many desktop publishing packages and web page editors now use Lorem Ipsum as their default model text, and a search for 'lorem ipsum' will uncover many web sites still in their infancy. Various versions have evolved over the years, sometimes by accident, sometimes on purpose (injected humour and the like).</t>
-  </si>
-  <si>
-    <t>Contrary to popular belief, Lorem Ipsum is not simply random text. It has roots in a piece of classical Latin literature from 45 BC, making it over 2000 years old. Richard McClintock, a Latin professor at Hampden-Sydney College in Virginia, looked up one of the more obscure Latin words, consectetur, from a Lorem Ipsum passage, and going through the cites of the word in classical literature, discovered the undoubtable source. Lorem Ipsum comes from sections 1.10.32 and 1.10.33 of "de Finibus Bonorum et Malorum" (The Extremes of Good and Evil) by Cicero, written in 45 BC. This book is a treatise on the theory of ethics, very popular during the Renaissance. The first line of Lorem Ipsum, "Lorem ipsum dolor sit amet..", comes from a line in section 1.10.32.</t>
-  </si>
-  <si>
-    <t>The standard chunk of Lorem Ipsum used since the 1500s is reproduced below for those interested. Sections 1.10.32 and 1.10.33 from "de Finibus Bonorum et Malorum" by Cicero are also reproduced in their exact original form, accompanied by English versions from the 1914 translation by H. Rackham.</t>
+    <t>James Bond</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF212529"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -114,25 +58,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -411,111 +343,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="23.85546875" customWidth="1"/>
-    <col min="2" max="2" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1">
+      <c r="A1" t="n">
+        <v>1001.0</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="n">
+        <v>89.0</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1002.0</v>
+      </c>
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A5"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="111" style="3" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" ht="103.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" ht="103.5" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>13</v>
+      <c r="C2" t="n">
+        <v>82.0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adding new CSV utility
</commit_message>
<xml_diff>
--- a/src/main/resources/testData/testData.xlsx
+++ b/src/main/resources/testData/testData.xlsx
@@ -19,12 +19,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="8">
   <si>
     <t>John Wick</t>
   </si>
   <si>
-    <t>James Bond</t>
+    <t>john@test.com</t>
+  </si>
+  <si>
+    <t>US</t>
+  </si>
+  <si>
+    <t>California</t>
+  </si>
+  <si>
+    <t>Sachin Taware</t>
+  </si>
+  <si>
+    <t>Sachin@Test.com</t>
+  </si>
+  <si>
+    <t>IND</t>
+  </si>
+  <si>
+    <t>Maharashtra</t>
   </si>
 </sst>
 </file>
@@ -61,8 +79,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -343,34 +370,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="n">
-        <v>1001.0</v>
-      </c>
-      <c r="B1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="n">
-        <v>89.0</v>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>1002.0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="n">
-        <v>82.0</v>
+      <c r="A2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>